<commit_message>
Add final verslag stuff
</commit_message>
<xml_diff>
--- a/CG.xlsx
+++ b/CG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\Hoger Onderwijs\Projecten\CG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB0FE0F-FFEA-42C3-80B8-F285DDBB885C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308BE84E-A1A4-46D6-A852-7D3C72B87329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C8FC2F09-786C-4F83-BF76-63AF1CCD04F2}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>LearnOpengGL volgen</t>
   </si>
   <si>
-    <t>Abstractie OpenGL in klasse</t>
-  </si>
-  <si>
     <t>Vloer tekenen (1 uur)</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>Video, verslag maken (3 uur)</t>
+  </si>
+  <si>
+    <t>Abstractie OpenGL in klasse (10 uur)</t>
   </si>
 </sst>
 </file>
@@ -303,12 +303,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,52 +354,16 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +683,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,238 +699,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="12" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="14" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="12" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="12" t="s">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="12" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="19"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="10" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="12" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="12" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="12" t="s">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="13"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="21"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="23"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
@@ -1069,25 +1069,11 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B11:B20"/>
-    <mergeCell ref="D11:D20"/>
-    <mergeCell ref="F11:F20"/>
-    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="E11:E12"/>
@@ -1104,11 +1090,25 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="D11:D20"/>
+    <mergeCell ref="F11:F20"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G19:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>